<commit_message>
Matriz de costos aprobada
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.1.xlsx
+++ b/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
   <si>
     <t>Estimación de Costos</t>
   </si>
@@ -344,9 +344,6 @@
     <t>Celular LG-G4  4G</t>
   </si>
   <si>
-    <t>Telefonica Celular</t>
-  </si>
-  <si>
     <t>Alquiler</t>
   </si>
   <si>
@@ -375,6 +372,12 @@
   </si>
   <si>
     <t>Equipamiento</t>
+  </si>
+  <si>
+    <t>Telefonia Celular</t>
+  </si>
+  <si>
+    <t>Telefonia celular para Project manager y Project Leader.</t>
   </si>
 </sst>
 </file>
@@ -1235,6 +1238,37 @@
     <xf numFmtId="166" fontId="10" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,11 +1290,18 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1281,44 +1322,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1691,7 +1694,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1701,8 +1704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1717,22 +1720,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="100"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1744,11 +1747,11 @@
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
       <c r="D2" s="78"/>
       <c r="E2" s="75" t="s">
         <v>69</v>
@@ -1791,10 +1794,10 @@
       <c r="W2" s="4"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="96" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1848,8 +1851,8 @@
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="94"/>
-      <c r="B4" s="92"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="108"/>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1901,8 +1904,8 @@
       <c r="V4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94"/>
-      <c r="B5" s="85" t="s">
+      <c r="A5" s="106"/>
+      <c r="B5" s="96" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1929,8 +1932,8 @@
       <c r="V5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="94"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1955,8 +1958,8 @@
       <c r="V6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="94"/>
-      <c r="B7" s="85" t="s">
+      <c r="A7" s="106"/>
+      <c r="B7" s="96" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -1983,8 +1986,8 @@
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="94"/>
-      <c r="B8" s="92"/>
+      <c r="A8" s="106"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
@@ -2009,8 +2012,8 @@
       <c r="V8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="94"/>
-      <c r="B9" s="85" t="s">
+      <c r="A9" s="106"/>
+      <c r="B9" s="96" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2039,8 +2042,8 @@
       <c r="V9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="94"/>
-      <c r="B10" s="92"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="108"/>
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
@@ -2083,7 +2086,7 @@
       <c r="V10" s="9"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="94"/>
+      <c r="A11" s="106"/>
       <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E11" s="77">
         <v>1500</v>
@@ -2120,7 +2123,9 @@
       <c r="M11" s="77">
         <v>1500</v>
       </c>
-      <c r="N11" s="6"/>
+      <c r="N11" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -2131,12 +2136,12 @@
       <c r="V11" s="9"/>
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="94"/>
-      <c r="B12" s="85" t="s">
+      <c r="A12" s="106"/>
+      <c r="B12" s="96" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="77">
@@ -2177,49 +2182,49 @@
       <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="94"/>
-      <c r="B13" s="86"/>
+      <c r="A13" s="106"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="83"/>
-      <c r="E13" s="104">
+      <c r="E13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="F13" s="104">
+      <c r="F13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="G13" s="104">
+      <c r="G13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="H13" s="104">
+      <c r="H13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="I13" s="104">
+      <c r="I13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="J13" s="104">
+      <c r="J13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="K13" s="104">
+      <c r="K13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="L13" s="104">
+      <c r="L13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="M13" s="104">
+      <c r="M13" s="87">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="N13" s="105"/>
+      <c r="N13" s="88"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
@@ -2230,26 +2235,26 @@
       <c r="V13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="109"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="109"/>
-      <c r="J14" s="109"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="109"/>
-      <c r="N14" s="109"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
@@ -2260,22 +2265,22 @@
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="110"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="108" t="s">
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="108"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="109"/>
-      <c r="N15" s="109"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
@@ -2286,24 +2291,24 @@
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="110"/>
-      <c r="B16" s="107" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="C16" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
-      <c r="I16" s="109"/>
-      <c r="J16" s="109"/>
-      <c r="K16" s="109"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="109"/>
-      <c r="N16" s="109"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
@@ -2314,22 +2319,22 @@
       <c r="V16" s="9"/>
     </row>
     <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="110"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="108" t="s">
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="108"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109"/>
-      <c r="J17" s="109"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="109"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
@@ -2340,24 +2345,24 @@
       <c r="V17" s="9"/>
     </row>
     <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="110"/>
-      <c r="B18" s="107" t="s">
+      <c r="A18" s="104"/>
+      <c r="B18" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="108"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="109"/>
-      <c r="J18" s="109"/>
-      <c r="K18" s="109"/>
-      <c r="L18" s="109"/>
-      <c r="M18" s="109"/>
-      <c r="N18" s="109"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -2368,22 +2373,22 @@
       <c r="V18" s="9"/>
     </row>
     <row r="19" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="110"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="108" t="s">
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="108"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="109"/>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="90"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
@@ -2394,24 +2399,24 @@
       <c r="V19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="110"/>
-      <c r="B20" s="107" t="s">
+      <c r="A20" s="104"/>
+      <c r="B20" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="108" t="s">
+      <c r="C20" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="108"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="109"/>
-      <c r="J20" s="109"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="109"/>
-      <c r="N20" s="109"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -2422,22 +2427,22 @@
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="110"/>
-      <c r="B21" s="110"/>
-      <c r="C21" s="108" t="s">
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="90"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
@@ -2448,24 +2453,24 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="110"/>
-      <c r="B22" s="107" t="s">
+      <c r="A22" s="104"/>
+      <c r="B22" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="108"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="109"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
-      <c r="K22" s="109"/>
-      <c r="L22" s="109"/>
-      <c r="M22" s="109"/>
-      <c r="N22" s="109"/>
+      <c r="D22" s="89"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
@@ -2476,22 +2481,22 @@
       <c r="V22" s="9"/>
     </row>
     <row r="23" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="110"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="108" t="s">
+      <c r="A23" s="104"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="108"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
@@ -2502,24 +2507,24 @@
       <c r="V23" s="9"/>
     </row>
     <row r="24" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="110"/>
-      <c r="B24" s="107" t="s">
+      <c r="A24" s="104"/>
+      <c r="B24" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="109"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="109"/>
-      <c r="I24" s="109"/>
-      <c r="J24" s="109"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="109"/>
-      <c r="N24" s="109"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
@@ -2530,22 +2535,22 @@
       <c r="V24" s="9"/>
     </row>
     <row r="25" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="110"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="108" t="s">
+      <c r="A25" s="104"/>
+      <c r="B25" s="104"/>
+      <c r="C25" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="108"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
@@ -2556,55 +2561,55 @@
       <c r="V25" s="9"/>
     </row>
     <row r="26" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="114" t="s">
+      <c r="A26" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="114" t="s">
+      <c r="B26" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="89" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="89"/>
+      <c r="E26" s="91">
+        <v>36350</v>
+      </c>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+    </row>
+    <row r="27" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="95"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="108" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="108"/>
-      <c r="E26" s="111">
-        <v>36350</v>
-      </c>
-      <c r="F26" s="109"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
-      <c r="I26" s="109"/>
-      <c r="J26" s="109"/>
-      <c r="K26" s="109"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="109"/>
-    </row>
-    <row r="27" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="115"/>
-      <c r="B27" s="115"/>
-      <c r="C27" s="108" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="112"/>
-      <c r="E27" s="111">
+      <c r="D27" s="92"/>
+      <c r="E27" s="91">
         <v>156800</v>
       </c>
-      <c r="F27" s="113"/>
-      <c r="G27" s="113"/>
-      <c r="H27" s="113"/>
-      <c r="I27" s="113"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="113"/>
-      <c r="L27" s="113"/>
-      <c r="M27" s="113"/>
-      <c r="N27" s="112"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="92"/>
     </row>
     <row r="28" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="102"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="103"/>
+      <c r="E28" s="86"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -2619,7 +2624,7 @@
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="57" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" s="57"/>
       <c r="E29" s="57">
@@ -18243,6 +18248,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B12:B13"/>
@@ -18259,7 +18265,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18270,8 +18275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18805,17 +18810,17 @@
       <c r="B26" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="97" t="s">
+      <c r="C26" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="98"/>
-      <c r="H26" s="98"/>
-      <c r="I26" s="98"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="99"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="112"/>
+      <c r="F26" s="112"/>
+      <c r="G26" s="112"/>
+      <c r="H26" s="112"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
+      <c r="K26" s="113"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
@@ -19280,18 +19285,18 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="96"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="109"/>
+      <c r="F39" s="109"/>
+      <c r="G39" s="109"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="109"/>
+      <c r="J39" s="110"/>
       <c r="K39" s="42">
         <f>SUM(C35:K35)</f>
         <v>2478443.5199999996</v>
@@ -19387,10 +19392,10 @@
       <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="100"/>
+      <c r="B9" s="114"/>
       <c r="C9" s="48">
         <f>SUM(C3:C8)</f>
         <v>210000</v>
@@ -19658,10 +19663,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="115" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="101"/>
+      <c r="B18" s="115"/>
       <c r="C18" s="74"/>
       <c r="D18" s="48">
         <f>SUM(D4:D17)</f>
@@ -19759,10 +19764,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="115" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="115"/>
       <c r="C25" s="74"/>
       <c r="D25" s="48">
         <f>SUM(D19:D24)</f>
@@ -19770,10 +19775,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="101" t="s">
+      <c r="A26" s="115" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="101"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="74"/>
       <c r="D26" s="48">
         <f>D18+D25</f>
@@ -19805,7 +19810,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="79">
         <v>3500</v>
@@ -19813,7 +19818,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="79">
         <v>15000</v>
@@ -19821,7 +19826,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="79">
         <v>4000</v>
@@ -19829,7 +19834,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="79">
         <v>4000</v>
@@ -19837,7 +19842,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5" s="79">
         <v>10000</v>

</xml_diff>

<commit_message>
Actualizacion de informe de avance, Acta de Proyecto V1.6. Correcion en la matriz de costo en la seccion de RRHH que no calculaba bien el total
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.1.xlsx
+++ b/trunk/docs/Entregables/Matriz de Costos/Plantilla Estimación de Costos v1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimación de Costos" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1025,6 +1025,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1032,7 +1043,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1121,9 +1132,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1247,9 +1255,6 @@
     <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1263,6 +1268,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1290,10 +1299,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1321,6 +1326,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1694,7 +1706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1704,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1752,35 +1764,35 @@
       </c>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="75" t="s">
+      <c r="D2" s="77"/>
+      <c r="E2" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="76" t="s">
+      <c r="F2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="I2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="76" t="s">
+      <c r="J2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="75" t="s">
+      <c r="K2" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="76" t="s">
+      <c r="L2" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="72" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="2"/>
@@ -1794,7 +1806,7 @@
       <c r="W2" s="4"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="103" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="96" t="s">
@@ -1804,43 +1816,43 @@
         <v>13</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="80">
+      <c r="E3" s="79">
         <f>RRHH!C35</f>
         <v>193628.4</v>
       </c>
-      <c r="F3" s="80">
+      <c r="F3" s="79">
         <f>RRHH!D35</f>
         <v>193628.4</v>
       </c>
-      <c r="G3" s="80">
+      <c r="G3" s="79">
         <f>RRHH!E35</f>
         <v>242035.5</v>
       </c>
-      <c r="H3" s="80">
+      <c r="H3" s="79">
         <f>RRHH!F35</f>
         <v>360148.82399999996</v>
       </c>
-      <c r="I3" s="80">
+      <c r="I3" s="79">
         <f>RRHH!G35</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="J3" s="80">
+      <c r="J3" s="79">
         <f>RRHH!H35</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="K3" s="80">
+      <c r="K3" s="79">
         <f>RRHH!I35</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="L3" s="80">
+      <c r="L3" s="79">
         <f>RRHH!J35</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="M3" s="80">
+      <c r="M3" s="79">
         <f>RRHH!K35</f>
         <v>273016.04399999999</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="114"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
@@ -1851,45 +1863,45 @@
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="106"/>
-      <c r="B4" s="108"/>
+      <c r="A4" s="104"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="80">
+      <c r="E4" s="79">
         <f>RRHH!B36</f>
         <v>0</v>
       </c>
-      <c r="F4" s="80">
+      <c r="F4" s="79">
         <f>RRHH!C36</f>
         <v>0</v>
       </c>
-      <c r="G4" s="80">
+      <c r="G4" s="79">
         <f>RRHH!D36</f>
         <v>0</v>
       </c>
-      <c r="H4" s="80">
+      <c r="H4" s="79">
         <f>RRHH!E36</f>
         <v>40000</v>
       </c>
-      <c r="I4" s="80">
+      <c r="I4" s="79">
         <f>RRHH!F36</f>
         <v>40000</v>
       </c>
-      <c r="J4" s="80">
+      <c r="J4" s="79">
         <f>RRHH!G36</f>
         <v>40000</v>
       </c>
-      <c r="K4" s="80">
+      <c r="K4" s="79">
         <f>RRHH!H36</f>
         <v>40000</v>
       </c>
-      <c r="L4" s="80">
+      <c r="L4" s="79">
         <f>RRHH!I36</f>
         <v>0</v>
       </c>
-      <c r="M4" s="80">
+      <c r="M4" s="79">
         <f>RRHH!J36</f>
         <v>0</v>
       </c>
@@ -1904,7 +1916,7 @@
       <c r="V4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="106"/>
+      <c r="A5" s="104"/>
       <c r="B5" s="96" t="s">
         <v>15</v>
       </c>
@@ -1932,8 +1944,8 @@
       <c r="V5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="106"/>
-      <c r="B6" s="108"/>
+      <c r="A6" s="104"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1958,7 +1970,7 @@
       <c r="V6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="96" t="s">
         <v>16</v>
       </c>
@@ -1986,8 +1998,8 @@
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="106"/>
-      <c r="B8" s="108"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="106"/>
       <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
@@ -2012,7 +2024,7 @@
       <c r="V8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="106"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="96" t="s">
         <v>19</v>
       </c>
@@ -2020,7 +2032,7 @@
         <v>20</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="77">
+      <c r="E9" s="76">
         <v>210000</v>
       </c>
       <c r="F9" s="6"/>
@@ -2042,40 +2054,40 @@
       <c r="V9" s="9"/>
     </row>
     <row r="10" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="106"/>
-      <c r="B10" s="108"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="77">
+      <c r="E10" s="76">
         <v>20000</v>
       </c>
-      <c r="F10" s="77">
+      <c r="F10" s="76">
         <v>20000</v>
       </c>
-      <c r="G10" s="77">
+      <c r="G10" s="76">
         <v>20000</v>
       </c>
-      <c r="H10" s="77">
+      <c r="H10" s="76">
         <v>20000</v>
       </c>
-      <c r="I10" s="77">
+      <c r="I10" s="76">
         <v>20000</v>
       </c>
-      <c r="J10" s="77">
+      <c r="J10" s="76">
         <v>20000</v>
       </c>
-      <c r="K10" s="77">
+      <c r="K10" s="76">
         <v>20000</v>
       </c>
-      <c r="L10" s="77">
+      <c r="L10" s="76">
         <v>20000</v>
       </c>
-      <c r="M10" s="77">
+      <c r="M10" s="76">
         <v>20000</v>
       </c>
-      <c r="N10" s="6"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -2086,7 +2098,7 @@
       <c r="V10" s="9"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="106"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
@@ -2096,31 +2108,31 @@
       <c r="D11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="77">
+      <c r="E11" s="76">
         <v>1500</v>
       </c>
-      <c r="F11" s="77">
+      <c r="F11" s="76">
         <v>1500</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="76">
         <v>1500</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="76">
         <v>1500</v>
       </c>
-      <c r="I11" s="77">
+      <c r="I11" s="76">
         <v>1500</v>
       </c>
-      <c r="J11" s="77">
+      <c r="J11" s="76">
         <v>1500</v>
       </c>
-      <c r="K11" s="77">
+      <c r="K11" s="76">
         <v>1500</v>
       </c>
-      <c r="L11" s="77">
+      <c r="L11" s="76">
         <v>1500</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="76">
         <v>1500</v>
       </c>
       <c r="N11" s="6" t="s">
@@ -2136,7 +2148,7 @@
       <c r="V11" s="9"/>
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="106"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="96" t="s">
         <v>24</v>
       </c>
@@ -2144,34 +2156,34 @@
         <v>108</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="77">
+      <c r="E12" s="76">
         <v>50000</v>
       </c>
-      <c r="F12" s="77">
+      <c r="F12" s="76">
         <v>50000</v>
       </c>
-      <c r="G12" s="77">
+      <c r="G12" s="76">
         <v>50000</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="76">
         <v>50000</v>
       </c>
-      <c r="I12" s="77">
+      <c r="I12" s="76">
         <v>50000</v>
       </c>
-      <c r="J12" s="77">
+      <c r="J12" s="76">
         <v>50000</v>
       </c>
-      <c r="K12" s="77">
+      <c r="K12" s="76">
         <v>50000</v>
       </c>
-      <c r="L12" s="77">
+      <c r="L12" s="76">
         <v>50000</v>
       </c>
-      <c r="M12" s="77">
+      <c r="M12" s="76">
         <v>50000</v>
       </c>
-      <c r="N12" s="6"/>
+      <c r="N12" s="76"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
@@ -2182,49 +2194,49 @@
       <c r="V12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="106"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="97"/>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="83"/>
-      <c r="E13" s="87">
+      <c r="D13" s="82"/>
+      <c r="E13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="G13" s="87">
+      <c r="G13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="H13" s="87">
+      <c r="H13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="I13" s="87">
+      <c r="I13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="J13" s="87">
+      <c r="J13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="K13" s="87">
+      <c r="K13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="L13" s="87">
+      <c r="L13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="M13" s="87">
+      <c r="M13" s="86">
         <f>'Impuestos y Servicios'!$B$6</f>
         <v>36500</v>
       </c>
-      <c r="N13" s="88"/>
+      <c r="N13" s="86"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
@@ -2235,26 +2247,26 @@
       <c r="V13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="107" t="s">
+      <c r="A14" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="8"/>
@@ -2265,22 +2277,22 @@
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="104"/>
-      <c r="C15" s="89" t="s">
+      <c r="A15" s="93"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
@@ -2291,24 +2303,24 @@
       <c r="V15" s="9"/>
     </row>
     <row r="16" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="89" t="s">
+      <c r="C16" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="89"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="88"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="88"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="88"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
@@ -2319,22 +2331,22 @@
       <c r="V16" s="9"/>
     </row>
     <row r="17" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="104"/>
-      <c r="C17" s="89" t="s">
+      <c r="A17" s="93"/>
+      <c r="B17" s="93"/>
+      <c r="C17" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="90"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="88"/>
+      <c r="H17" s="88"/>
+      <c r="I17" s="88"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="88"/>
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
@@ -2345,24 +2357,24 @@
       <c r="V17" s="9"/>
     </row>
     <row r="18" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="103" t="s">
+      <c r="A18" s="93"/>
+      <c r="B18" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="89" t="s">
+      <c r="C18" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="88"/>
+      <c r="N18" s="88"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
@@ -2373,22 +2385,22 @@
       <c r="V18" s="9"/>
     </row>
     <row r="19" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="104"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="89" t="s">
+      <c r="A19" s="93"/>
+      <c r="B19" s="93"/>
+      <c r="C19" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="89"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="90"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="90"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="88"/>
+      <c r="N19" s="88"/>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
@@ -2399,24 +2411,24 @@
       <c r="V19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="103" t="s">
+      <c r="A20" s="93"/>
+      <c r="B20" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="89" t="s">
+      <c r="C20" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="89"/>
-      <c r="E20" s="90"/>
-      <c r="F20" s="90"/>
-      <c r="G20" s="90"/>
-      <c r="H20" s="90"/>
-      <c r="I20" s="90"/>
-      <c r="J20" s="90"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="90"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
@@ -2427,22 +2439,22 @@
       <c r="V20" s="9"/>
     </row>
     <row r="21" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
-      <c r="B21" s="104"/>
-      <c r="C21" s="89" t="s">
+      <c r="A21" s="93"/>
+      <c r="B21" s="93"/>
+      <c r="C21" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="89"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="90"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="90"/>
-      <c r="J21" s="90"/>
-      <c r="K21" s="90"/>
-      <c r="L21" s="90"/>
-      <c r="M21" s="90"/>
-      <c r="N21" s="90"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
@@ -2453,24 +2465,24 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="103" t="s">
+      <c r="A22" s="93"/>
+      <c r="B22" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C22" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="89"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="90"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="90"/>
-      <c r="K22" s="90"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="90"/>
-      <c r="N22" s="90"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="88"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="88"/>
+      <c r="I22" s="88"/>
+      <c r="J22" s="88"/>
+      <c r="K22" s="88"/>
+      <c r="L22" s="88"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
@@ -2481,22 +2493,22 @@
       <c r="V22" s="9"/>
     </row>
     <row r="23" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="89" t="s">
+      <c r="A23" s="93"/>
+      <c r="B23" s="93"/>
+      <c r="C23" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="89"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="90"/>
-      <c r="J23" s="90"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="90"/>
-      <c r="N23" s="90"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="88"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="88"/>
+      <c r="L23" s="88"/>
+      <c r="M23" s="88"/>
+      <c r="N23" s="88"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
@@ -2507,24 +2519,24 @@
       <c r="V23" s="9"/>
     </row>
     <row r="24" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="103" t="s">
+      <c r="A24" s="93"/>
+      <c r="B24" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="89" t="s">
+      <c r="C24" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="89"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
-      <c r="J24" s="90"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
@@ -2535,22 +2547,22 @@
       <c r="V24" s="9"/>
     </row>
     <row r="25" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
-      <c r="B25" s="104"/>
-      <c r="C25" s="89" t="s">
+      <c r="A25" s="93"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
@@ -2567,49 +2579,49 @@
       <c r="B26" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="89"/>
-      <c r="E26" s="91">
+      <c r="D26" s="87"/>
+      <c r="E26" s="89">
         <v>36350</v>
       </c>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="90"/>
-      <c r="N26" s="90"/>
+      <c r="F26" s="88"/>
+      <c r="G26" s="88"/>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+      <c r="K26" s="88"/>
+      <c r="L26" s="88"/>
+      <c r="M26" s="88"/>
+      <c r="N26" s="88"/>
     </row>
     <row r="27" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="95"/>
       <c r="B27" s="95"/>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="92"/>
-      <c r="E27" s="91">
+      <c r="D27" s="90"/>
+      <c r="E27" s="89">
         <v>156800</v>
       </c>
-      <c r="F27" s="93"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
-      <c r="K27" s="93"/>
-      <c r="L27" s="93"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="92"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="L27" s="91"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="90"/>
     </row>
     <row r="28" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="85"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="86"/>
+      <c r="E28" s="85"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -2623,43 +2635,43 @@
     <row r="29" spans="1:22" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57">
+      <c r="D29" s="56"/>
+      <c r="E29" s="56">
         <f>SUM(E3:E27)</f>
         <v>704778.4</v>
       </c>
-      <c r="F29" s="57">
+      <c r="F29" s="56">
         <f t="shared" ref="F29:L29" si="0">SUM(F3:F26)</f>
         <v>301628.40000000002</v>
       </c>
-      <c r="G29" s="57">
+      <c r="G29" s="56">
         <f t="shared" si="0"/>
         <v>350035.5</v>
       </c>
-      <c r="H29" s="57">
+      <c r="H29" s="56">
         <f t="shared" si="0"/>
         <v>508148.82399999996</v>
       </c>
-      <c r="I29" s="57">
+      <c r="I29" s="56">
         <f t="shared" si="0"/>
         <v>451996.58799999999</v>
       </c>
-      <c r="J29" s="57">
+      <c r="J29" s="56">
         <f t="shared" si="0"/>
         <v>451996.58799999999</v>
       </c>
-      <c r="K29" s="57">
+      <c r="K29" s="56">
         <f t="shared" si="0"/>
         <v>451996.58799999999</v>
       </c>
-      <c r="L29" s="57">
+      <c r="L29" s="56">
         <f t="shared" si="0"/>
         <v>411996.58799999999</v>
       </c>
-      <c r="M29" s="57">
+      <c r="M29" s="56">
         <f>SUM(M3:M26)</f>
         <v>381016.04399999999</v>
       </c>
@@ -2668,43 +2680,43 @@
     <row r="30" spans="1:22" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57">
+      <c r="D30" s="56"/>
+      <c r="E30" s="56">
         <f>E29</f>
         <v>704778.4</v>
       </c>
-      <c r="F30" s="57">
+      <c r="F30" s="56">
         <f>E30+F29</f>
         <v>1006406.8</v>
       </c>
-      <c r="G30" s="57">
+      <c r="G30" s="56">
         <f>F30+G29</f>
         <v>1356442.3</v>
       </c>
-      <c r="H30" s="57">
+      <c r="H30" s="56">
         <f t="shared" ref="H30:M30" si="1">G30+H29</f>
         <v>1864591.1240000001</v>
       </c>
-      <c r="I30" s="57">
+      <c r="I30" s="56">
         <f t="shared" si="1"/>
         <v>2316587.7120000003</v>
       </c>
-      <c r="J30" s="57">
+      <c r="J30" s="56">
         <f t="shared" si="1"/>
         <v>2768584.3000000003</v>
       </c>
-      <c r="K30" s="57">
+      <c r="K30" s="56">
         <f t="shared" si="1"/>
         <v>3220580.8880000003</v>
       </c>
-      <c r="L30" s="57">
+      <c r="L30" s="56">
         <f t="shared" si="1"/>
         <v>3632577.4760000003</v>
       </c>
-      <c r="M30" s="84">
+      <c r="M30" s="83">
         <f t="shared" si="1"/>
         <v>4013593.5200000005</v>
       </c>
@@ -18248,6 +18260,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
@@ -18264,7 +18277,6 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B14:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18273,10 +18285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K39"/>
+  <dimension ref="A2:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -18313,7 +18325,7 @@
       <c r="H3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="48" t="s">
         <v>44</v>
       </c>
     </row>
@@ -18340,12 +18352,12 @@
         <v>50</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="49" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="17">
@@ -18375,13 +18387,13 @@
         <f t="shared" ref="H5:H13" si="5">D5*$B$23</f>
         <v>2160.06</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="51">
         <f t="shared" ref="I5:I13" si="6">SUM(D5:H5)</f>
         <v>67769.94</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="50" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="17">
@@ -18411,13 +18423,13 @@
         <f t="shared" si="5"/>
         <v>1728.048</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="51">
         <f t="shared" si="6"/>
         <v>54215.951999999997</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="50" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="17">
@@ -18447,13 +18459,13 @@
         <f t="shared" si="5"/>
         <v>1542.9</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="51">
         <f t="shared" si="6"/>
         <v>48407.1</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="17">
@@ -18483,13 +18495,13 @@
         <f t="shared" si="5"/>
         <v>1542.9</v>
       </c>
-      <c r="I8" s="52">
+      <c r="I8" s="51">
         <f t="shared" si="6"/>
         <v>48407.1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="17">
@@ -18519,13 +18531,13 @@
         <f t="shared" si="5"/>
         <v>1234.32</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="51">
         <f t="shared" si="6"/>
         <v>38725.68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="17"/>
@@ -18535,12 +18547,12 @@
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
-      <c r="I10" s="53">
+      <c r="I10" s="52">
         <v>40000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="50" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="17">
@@ -18570,13 +18582,13 @@
         <f t="shared" si="5"/>
         <v>987.45600000000002</v>
       </c>
-      <c r="I11" s="53">
+      <c r="I11" s="52">
         <f t="shared" si="6"/>
         <v>30980.544000000002</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="17">
@@ -18606,13 +18618,13 @@
         <f t="shared" si="5"/>
         <v>1789.7640000000001</v>
       </c>
-      <c r="I12" s="53">
+      <c r="I12" s="52">
         <f t="shared" si="6"/>
         <v>56152.235999999997</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="53" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="17">
@@ -18642,44 +18654,44 @@
         <f t="shared" si="5"/>
         <v>493.72800000000001</v>
       </c>
-      <c r="I13" s="53">
+      <c r="I13" s="52">
         <f t="shared" si="6"/>
         <v>15490.272000000001</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="56">
+      <c r="B14" s="55">
         <f>SUM(B5:B13)</f>
         <v>186000</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="56">
         <f t="shared" ref="C14:I14" si="8">SUM(C5:C13)</f>
         <v>89280</v>
       </c>
-      <c r="D14" s="56">
+      <c r="D14" s="55">
         <f t="shared" si="8"/>
         <v>275280</v>
       </c>
-      <c r="E14" s="56">
+      <c r="E14" s="55">
         <f t="shared" si="8"/>
         <v>22930.824000000001</v>
       </c>
-      <c r="F14" s="56">
+      <c r="F14" s="55">
         <f t="shared" si="8"/>
         <v>22930.824000000001</v>
       </c>
-      <c r="G14" s="56">
+      <c r="G14" s="55">
         <f t="shared" si="8"/>
         <v>27528</v>
       </c>
-      <c r="H14" s="56">
+      <c r="H14" s="55">
         <f t="shared" si="8"/>
         <v>11479.175999999999</v>
       </c>
-      <c r="I14" s="58">
+      <c r="I14" s="57">
         <f t="shared" si="8"/>
         <v>400148.82399999996</v>
       </c>
@@ -18687,13 +18699,13 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="21"/>
@@ -18810,17 +18822,17 @@
       <c r="B26" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="111" t="s">
+      <c r="C26" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="112"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="112"/>
-      <c r="K26" s="113"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="111"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
@@ -19050,7 +19062,7 @@
       </c>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="30" t="s">
         <v>59</v>
       </c>
@@ -19079,7 +19091,7 @@
       <c r="J33" s="36"/>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="30" t="s">
         <v>60</v>
       </c>
@@ -19123,7 +19135,7 @@
         <v>15490.272000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
         <v>71</v>
       </c>
@@ -19131,43 +19143,44 @@
         <v>0</v>
       </c>
       <c r="C35" s="37">
-        <f t="shared" ref="C35:K35" si="16">SUM(C28:C34)</f>
+        <f>SUM(C28:C34)</f>
         <v>193628.4</v>
       </c>
       <c r="D35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(D28:D34)</f>
         <v>193628.4</v>
       </c>
       <c r="E35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(E28:E34)</f>
         <v>242035.5</v>
       </c>
       <c r="F35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(F28:F34)</f>
         <v>360148.82399999996</v>
       </c>
       <c r="G35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(G28:G34)</f>
         <v>303996.58799999999</v>
       </c>
       <c r="H35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(H28:H34)</f>
         <v>303996.58799999999</v>
       </c>
       <c r="I35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(I28:I34)</f>
         <v>303996.58799999999</v>
       </c>
       <c r="J35" s="37">
-        <f t="shared" si="16"/>
+        <f>SUM(J28:J34)</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="K35" s="38">
-        <f t="shared" si="16"/>
+      <c r="K35" s="37">
+        <f>SUM(K28:K34)</f>
         <v>273016.04399999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="116"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="29" t="s">
         <v>57</v>
       </c>
@@ -19179,127 +19192,127 @@
         <v>40000</v>
       </c>
       <c r="F36" s="36">
-        <f t="shared" ref="F36:H36" si="17">$I$10</f>
+        <f t="shared" ref="F36:H36" si="16">$I$10</f>
         <v>40000</v>
       </c>
       <c r="G36" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>40000</v>
       </c>
       <c r="H36" s="36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>40000</v>
       </c>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
       <c r="K36" s="36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="40">
+      <c r="B37" s="39">
         <f>SUM(B36)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="40">
-        <f t="shared" ref="C37:K37" si="18">SUM(C36)</f>
+      <c r="C37" s="39">
+        <f t="shared" ref="C37:K37" si="17">SUM(C36)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="40">
-        <f t="shared" si="18"/>
+      <c r="D37" s="39">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="E37" s="40">
-        <f t="shared" si="18"/>
+      <c r="E37" s="39">
+        <f t="shared" si="17"/>
         <v>40000</v>
       </c>
-      <c r="F37" s="40">
-        <f t="shared" si="18"/>
+      <c r="F37" s="39">
+        <f t="shared" si="17"/>
         <v>40000</v>
       </c>
-      <c r="G37" s="40">
-        <f t="shared" si="18"/>
+      <c r="G37" s="39">
+        <f t="shared" si="17"/>
         <v>40000</v>
       </c>
-      <c r="H37" s="40">
-        <f t="shared" si="18"/>
+      <c r="H37" s="39">
+        <f t="shared" si="17"/>
         <v>40000</v>
       </c>
-      <c r="I37" s="40">
-        <f t="shared" si="18"/>
+      <c r="I37" s="39">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="J37" s="40">
-        <f t="shared" si="18"/>
+      <c r="J37" s="39">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="K37" s="40">
-        <f t="shared" si="18"/>
+      <c r="K37" s="39">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+    <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="41">
+      <c r="B38" s="40">
         <f>B35+B37</f>
         <v>0</v>
       </c>
-      <c r="C38" s="41">
-        <f t="shared" ref="C38:K38" si="19">C35+C37</f>
+      <c r="C38" s="40">
+        <f>SUM(C35:C36)</f>
         <v>193628.4</v>
       </c>
-      <c r="D38" s="41">
-        <f t="shared" si="19"/>
+      <c r="D38" s="40">
+        <f>SUM(D35:D36)</f>
         <v>193628.4</v>
       </c>
-      <c r="E38" s="41">
-        <f t="shared" si="19"/>
+      <c r="E38" s="40">
+        <f>SUM(E35:E36)</f>
         <v>282035.5</v>
       </c>
-      <c r="F38" s="41">
-        <f t="shared" si="19"/>
+      <c r="F38" s="40">
+        <f>SUM(F35:F36)</f>
         <v>400148.82399999996</v>
       </c>
-      <c r="G38" s="41">
-        <f t="shared" si="19"/>
+      <c r="G38" s="40">
+        <f>SUM(G35:G36)</f>
         <v>343996.58799999999</v>
       </c>
-      <c r="H38" s="41">
-        <f t="shared" si="19"/>
+      <c r="H38" s="40">
+        <f>SUM(H35:H36)</f>
         <v>343996.58799999999</v>
       </c>
-      <c r="I38" s="41">
-        <f t="shared" si="19"/>
+      <c r="I38" s="40">
+        <f t="shared" ref="I38:K38" si="18">SUM(I35:I36)</f>
         <v>303996.58799999999</v>
       </c>
-      <c r="J38" s="41">
-        <f t="shared" si="19"/>
+      <c r="J38" s="40">
+        <f t="shared" si="18"/>
         <v>303996.58799999999</v>
       </c>
-      <c r="K38" s="41">
-        <f t="shared" si="19"/>
+      <c r="K38" s="40">
+        <f t="shared" si="18"/>
         <v>273016.04399999999</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="109" t="s">
+    <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="109"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="109"/>
-      <c r="E39" s="109"/>
-      <c r="F39" s="109"/>
-      <c r="G39" s="109"/>
-      <c r="H39" s="109"/>
-      <c r="I39" s="109"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="42">
-        <f>SUM(C35:K35)</f>
-        <v>2478443.5199999996</v>
+      <c r="B39" s="107"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="107"/>
+      <c r="F39" s="107"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="108"/>
+      <c r="K39" s="41">
+        <f>SUM(C38:K38)</f>
+        <v>2638443.5199999996</v>
       </c>
     </row>
   </sheetData>
@@ -19317,7 +19330,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19339,18 +19352,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="44">
         <v>158000</v>
       </c>
     </row>
@@ -19358,10 +19371,10 @@
       <c r="A4" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="44">
         <v>12000</v>
       </c>
     </row>
@@ -19369,34 +19382,34 @@
       <c r="A5" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="46">
         <v>40000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="48">
+      <c r="B9" s="112"/>
+      <c r="C9" s="47">
         <f>SUM(C3:C8)</f>
         <v>210000</v>
       </c>
@@ -19431,356 +19444,356 @@
       <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="68" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="72"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="71"/>
     </row>
     <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="60">
+      <c r="B4" s="59">
         <v>1500</v>
       </c>
-      <c r="C4" s="61">
+      <c r="C4" s="60">
         <v>5</v>
       </c>
-      <c r="D4" s="81">
+      <c r="D4" s="80">
         <f t="shared" ref="D4:D17" si="0">B4*C4</f>
         <v>7500</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="59">
         <v>400</v>
       </c>
-      <c r="C5" s="61">
+      <c r="C5" s="60">
         <v>1</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="81">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="59">
         <v>450</v>
       </c>
-      <c r="C6" s="61">
+      <c r="C6" s="60">
         <v>1</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="81">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <v>1500</v>
       </c>
-      <c r="C7" s="61">
+      <c r="C7" s="60">
         <v>1</v>
       </c>
-      <c r="D7" s="82">
+      <c r="D7" s="81">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="60">
+      <c r="B8" s="59">
         <v>4200</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="60">
         <v>1</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="81">
         <f t="shared" si="0"/>
         <v>4200</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="60">
+      <c r="B9" s="59">
         <v>2000</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="60">
         <v>1</v>
       </c>
-      <c r="D9" s="82">
+      <c r="D9" s="81">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="60">
+      <c r="B10" s="59">
         <v>900</v>
       </c>
-      <c r="C10" s="61">
+      <c r="C10" s="60">
         <v>5</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="81">
         <f t="shared" si="0"/>
         <v>4500</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="60">
+      <c r="B11" s="59">
         <v>5000</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C11" s="60">
         <v>1</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="81">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="60">
+      <c r="B12" s="59">
         <v>1000</v>
       </c>
-      <c r="C12" s="61">
+      <c r="C12" s="60">
         <v>1</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="81">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="60">
+      <c r="B13" s="59">
         <v>700</v>
       </c>
-      <c r="C13" s="61">
+      <c r="C13" s="60">
         <v>5</v>
       </c>
-      <c r="D13" s="82">
+      <c r="D13" s="81">
         <f t="shared" si="0"/>
         <v>3500</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="60">
+      <c r="B14" s="59">
         <v>1500</v>
       </c>
-      <c r="C14" s="61">
+      <c r="C14" s="60">
         <v>1</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="81">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="60">
+      <c r="B15" s="59">
         <v>200</v>
       </c>
-      <c r="C15" s="61">
+      <c r="C15" s="60">
         <v>5</v>
       </c>
-      <c r="D15" s="82">
+      <c r="D15" s="81">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="60">
+      <c r="B16" s="59">
         <v>1600</v>
       </c>
-      <c r="C16" s="61">
+      <c r="C16" s="60">
         <v>2</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D16" s="81">
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="59">
         <v>600</v>
       </c>
-      <c r="C17" s="61">
+      <c r="C17" s="60">
         <v>1</v>
       </c>
-      <c r="D17" s="82">
+      <c r="D17" s="81">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="113" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="48">
+      <c r="B18" s="113"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="47">
         <f>SUM(D4:D17)</f>
         <v>36350</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="60">
+      <c r="B19" s="59">
         <v>19000</v>
       </c>
-      <c r="C19" s="61">
+      <c r="C19" s="60">
         <v>5</v>
       </c>
-      <c r="D19" s="60">
+      <c r="D19" s="59">
         <f t="shared" ref="D19:D24" si="1">B19*C19</f>
         <v>95000</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="59">
         <v>5500</v>
       </c>
-      <c r="C20" s="61">
+      <c r="C20" s="60">
         <v>1</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="59">
         <f t="shared" si="1"/>
         <v>5500</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="60">
+      <c r="B21" s="59">
         <v>1800</v>
       </c>
-      <c r="C21" s="61">
+      <c r="C21" s="60">
         <v>1</v>
       </c>
-      <c r="D21" s="60">
+      <c r="D21" s="59">
         <f t="shared" si="1"/>
         <v>1800</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="60">
+      <c r="B22" s="59">
         <v>40000</v>
       </c>
-      <c r="C22" s="61">
+      <c r="C22" s="60">
         <v>1</v>
       </c>
-      <c r="D22" s="60">
+      <c r="D22" s="59">
         <f t="shared" si="1"/>
         <v>40000</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="64">
+      <c r="B23" s="63">
         <v>9000</v>
       </c>
-      <c r="C23" s="65">
+      <c r="C23" s="64">
         <v>1</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="63">
         <f t="shared" si="1"/>
         <v>9000</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="64">
+      <c r="B24" s="63">
         <v>5500</v>
       </c>
-      <c r="C24" s="65">
+      <c r="C24" s="64">
         <v>1</v>
       </c>
-      <c r="D24" s="64">
+      <c r="D24" s="63">
         <f t="shared" si="1"/>
         <v>5500</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="115" t="s">
+      <c r="A25" s="113" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="115"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="48">
+      <c r="B25" s="113"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="47">
         <f>SUM(D19:D24)</f>
         <v>156800</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="113" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="48">
+      <c r="B26" s="113"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="47">
         <f>D18+D25</f>
         <v>193150</v>
       </c>
@@ -19800,7 +19813,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19809,50 +19822,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="79">
+      <c r="B1" s="78">
         <v>3500</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="79">
+      <c r="B2" s="78">
         <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="79">
+      <c r="B3" s="78">
         <v>4000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="79">
+      <c r="B4" s="78">
         <v>4000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="78">
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="47">
         <f>SUM(B1:B5)</f>
         <v>36500</v>
       </c>

</xml_diff>